<commit_message>
MAJOR update repo - new data and analysis
</commit_message>
<xml_diff>
--- a/data/selected_networks.xlsx
+++ b/data/selected_networks.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elena/Documents/EBD-PhD/individual_webs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaqb/Documents/EBD-PhD/individual_webs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DA1E10-831B-5D4B-B16C-D9C145CE5F63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41474B29-7057-DE40-9108-69259C9FD12F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="50080" windowHeight="28300" xr2:uid="{807D6CA5-9752-0F4A-B898-EE9DF220D9DC}"/>
+    <workbookView xWindow="1200" yWindow="12000" windowWidth="50000" windowHeight="16800" xr2:uid="{807D6CA5-9752-0F4A-B898-EE9DF220D9DC}"/>
   </bookViews>
   <sheets>
     <sheet name="webs" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">webs!$C$1:$L$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">webs!$C$1:$L$61</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="417">
   <si>
     <t>type</t>
   </si>
@@ -1336,6 +1336,27 @@
   <si>
     <t>Forest interior  (Netwrok B)</t>
   </si>
+  <si>
+    <t>21_02</t>
+  </si>
+  <si>
+    <t>Jayanth et al 2024 Biotropica</t>
+  </si>
+  <si>
+    <t>Naringi crenulata</t>
+  </si>
+  <si>
+    <t>Rutaceae</t>
+  </si>
+  <si>
+    <t>Mudumalai Tiger Reserve</t>
+  </si>
+  <si>
+    <t>Jayanth, A., Isvaran, K., &amp; Naniwadekar, R. (2024). Drivers of intraspecific variation in seed dispersal can differ across two species of fleshy-fruited savanna plants. Biotropica, 56(3), e13322. https://doi.org/10.1111/btp.13322</t>
+  </si>
+  <si>
+    <t>Jayanth, A., Isvaran, K., &amp; Naniwadekar, R. (2024). Drivers of intraspecific variation in seed dispersal can differ across two species of fleshy-fruited savanna plants. Biotropica, 56(3), e13322. https://doi.org/10.1111/btp.13323</t>
+  </si>
 </sst>
 </file>
 
@@ -1845,11 +1866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2128925D-BD8B-3641-9FF3-EAC703B2A479}">
-  <dimension ref="A1:U117"/>
+  <dimension ref="A1:U119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J119" sqref="J119"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M50" sqref="M50:M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3700,16 +3721,16 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="8" t="s">
         <v>376</v>
       </c>
       <c r="E48" s="7" t="s">
@@ -3738,16 +3759,16 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="8" t="s">
         <v>217</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="8" t="s">
         <v>377</v>
       </c>
       <c r="E49" s="23" t="s">
@@ -3777,42 +3798,78 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>69</v>
+        <v>218</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>275</v>
+        <v>411</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="H50" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>267</v>
+        <v>109</v>
+      </c>
+      <c r="I50" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="J50" s="14">
+        <v>11.55</v>
+      </c>
+      <c r="K50" s="14">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>205</v>
+        <v>415</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>70</v>
+        <v>202</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>410</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>275</v>
+        <v>411</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="H51" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>268</v>
+        <v>109</v>
+      </c>
+      <c r="I51" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="J51" s="14">
+        <v>11.55</v>
+      </c>
+      <c r="K51" s="14">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>205</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -3820,16 +3877,20 @@
         <v>204</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>286</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D52" s="8"/>
       <c r="H52" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="M52" s="8" t="s">
-        <v>276</v>
+      <c r="I52" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -3837,28 +3898,37 @@
         <v>204</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>281</v>
+        <v>275</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="H53" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="N53" s="8"/>
+        <v>205</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="M54" s="7" t="s">
-        <v>206</v>
+        <v>286</v>
+      </c>
+      <c r="H54" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -3866,7 +3936,7 @@
         <v>204</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>281</v>
@@ -3874,13 +3944,14 @@
       <c r="M55" s="7" t="s">
         <v>206</v>
       </c>
+      <c r="N55" s="8"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>281</v>
@@ -3894,13 +3965,13 @@
         <v>204</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M57" s="7" t="s">
-        <v>277</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -3908,13 +3979,13 @@
         <v>204</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>193</v>
+        <v>77</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="M58" s="8" t="s">
-        <v>207</v>
+        <v>281</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -3922,13 +3993,13 @@
         <v>204</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="M59" s="8" t="s">
-        <v>208</v>
+        <v>282</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -3936,13 +4007,13 @@
         <v>204</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>278</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -3950,13 +4021,13 @@
         <v>204</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="M61" s="7" t="s">
-        <v>209</v>
+        <v>88</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -3964,13 +4035,13 @@
         <v>204</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="M62" s="7" t="s">
-        <v>279</v>
+        <v>99</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="M62" s="8" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -3978,13 +4049,13 @@
         <v>204</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>290</v>
+        <v>104</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>288</v>
       </c>
       <c r="M63" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -3992,13 +4063,13 @@
         <v>204</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M64" s="7" t="s">
-        <v>211</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -4006,13 +4077,13 @@
         <v>204</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>292</v>
+        <v>125</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>290</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -4020,13 +4091,13 @@
         <v>204</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M66" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4034,13 +4105,13 @@
         <v>204</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="M67" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4048,49 +4119,35 @@
         <v>204</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>382</v>
+        <v>293</v>
       </c>
       <c r="M68" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="N68" s="8"/>
+        <v>213</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>269</v>
+        <v>153</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="I69" s="7" t="s">
-        <v>383</v>
+        <v>294</v>
       </c>
       <c r="M69" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="N69" s="8"/>
+        <v>214</v>
+      </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>270</v>
+        <v>158</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>296</v>
@@ -4099,7 +4156,7 @@
         <v>386</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>295</v>
@@ -4111,7 +4168,7 @@
         <v>204</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>296</v>
@@ -4120,7 +4177,7 @@
         <v>386</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M71" s="7" t="s">
         <v>295</v>
@@ -4132,57 +4189,71 @@
         <v>204</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>297</v>
+        <v>270</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>384</v>
       </c>
       <c r="M72" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+      <c r="N72" s="8"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="J73" s="24"/>
-      <c r="K73" s="24"/>
-      <c r="M73" s="8" t="s">
-        <v>216</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="M73" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="N73" s="8"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M74" s="8" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="M75" s="7" t="s">
-        <v>301</v>
+        <v>169</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="M75" s="8" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4190,13 +4261,13 @@
         <v>204</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="M76" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="M76" s="8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4204,13 +4275,13 @@
         <v>204</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="M77" s="7" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -4218,13 +4289,13 @@
         <v>204</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M78" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4232,13 +4303,13 @@
         <v>204</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="M79" s="8" t="s">
-        <v>308</v>
+        <v>218</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="M79" s="7" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4246,13 +4317,13 @@
         <v>204</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>311</v>
+        <v>219</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="M80" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -4260,19 +4331,13 @@
         <v>204</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="M81" s="7" t="s">
-        <v>312</v>
+        <v>220</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="M81" s="8" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -4280,19 +4345,13 @@
         <v>204</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I82" s="7" t="s">
-        <v>388</v>
+        <v>221</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>311</v>
       </c>
       <c r="M82" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
@@ -4300,7 +4359,7 @@
         <v>204</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>313</v>
@@ -4309,7 +4368,7 @@
         <v>93</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="M83" s="7" t="s">
         <v>312</v>
@@ -4320,13 +4379,19 @@
         <v>204</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>388</v>
       </c>
       <c r="M84" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -4334,13 +4399,19 @@
         <v>204</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>402</v>
       </c>
       <c r="M85" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
@@ -4348,13 +4419,13 @@
         <v>204</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="M86" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -4362,19 +4433,13 @@
         <v>204</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I87" s="7" t="s">
-        <v>389</v>
+        <v>317</v>
       </c>
       <c r="M87" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -4382,19 +4447,13 @@
         <v>204</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="H88" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I88" s="7" t="s">
-        <v>390</v>
+        <v>319</v>
       </c>
       <c r="M88" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -4402,7 +4461,7 @@
         <v>204</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>321</v>
@@ -4410,8 +4469,8 @@
       <c r="H89" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I89" s="12" t="s">
-        <v>391</v>
+      <c r="I89" s="7" t="s">
+        <v>389</v>
       </c>
       <c r="M89" s="7" t="s">
         <v>320</v>
@@ -4422,7 +4481,7 @@
         <v>204</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>321</v>
@@ -4430,8 +4489,8 @@
       <c r="H90" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I90" s="12" t="s">
-        <v>392</v>
+      <c r="I90" s="7" t="s">
+        <v>390</v>
       </c>
       <c r="M90" s="7" t="s">
         <v>320</v>
@@ -4442,7 +4501,7 @@
         <v>204</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>321</v>
@@ -4450,8 +4509,8 @@
       <c r="H91" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I91" s="7" t="s">
-        <v>393</v>
+      <c r="I91" s="12" t="s">
+        <v>391</v>
       </c>
       <c r="M91" s="7" t="s">
         <v>320</v>
@@ -4462,7 +4521,7 @@
         <v>204</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>321</v>
@@ -4470,8 +4529,8 @@
       <c r="H92" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I92" s="7" t="s">
-        <v>394</v>
+      <c r="I92" s="12" t="s">
+        <v>392</v>
       </c>
       <c r="M92" s="7" t="s">
         <v>320</v>
@@ -4482,7 +4541,7 @@
         <v>204</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>321</v>
@@ -4491,7 +4550,7 @@
         <v>403</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M93" s="7" t="s">
         <v>320</v>
@@ -4502,7 +4561,7 @@
         <v>204</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>321</v>
@@ -4511,7 +4570,7 @@
         <v>403</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M94" s="7" t="s">
         <v>320</v>
@@ -4522,7 +4581,7 @@
         <v>204</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>321</v>
@@ -4530,8 +4589,8 @@
       <c r="H95" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I95" s="12" t="s">
-        <v>397</v>
+      <c r="I95" s="7" t="s">
+        <v>395</v>
       </c>
       <c r="M95" s="7" t="s">
         <v>320</v>
@@ -4542,7 +4601,7 @@
         <v>204</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>321</v>
@@ -4551,7 +4610,7 @@
         <v>403</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M96" s="7" t="s">
         <v>320</v>
@@ -4562,7 +4621,7 @@
         <v>204</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>321</v>
@@ -4570,8 +4629,8 @@
       <c r="H97" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I97" s="7" t="s">
-        <v>399</v>
+      <c r="I97" s="12" t="s">
+        <v>397</v>
       </c>
       <c r="M97" s="7" t="s">
         <v>320</v>
@@ -4582,7 +4641,7 @@
         <v>204</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>321</v>
@@ -4591,7 +4650,7 @@
         <v>403</v>
       </c>
       <c r="I98" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M98" s="7" t="s">
         <v>320</v>
@@ -4602,7 +4661,7 @@
         <v>204</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>321</v>
@@ -4611,7 +4670,7 @@
         <v>403</v>
       </c>
       <c r="I99" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M99" s="7" t="s">
         <v>320</v>
@@ -4622,13 +4681,19 @@
         <v>204</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>322</v>
+        <v>239</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="H100" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I100" s="7" t="s">
+        <v>400</v>
       </c>
       <c r="M100" s="7" t="s">
-        <v>241</v>
+        <v>320</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -4636,13 +4701,19 @@
         <v>204</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>401</v>
       </c>
       <c r="M101" s="7" t="s">
-        <v>243</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -4650,13 +4721,13 @@
         <v>204</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>324</v>
+        <v>242</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>322</v>
       </c>
       <c r="M102" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -4664,13 +4735,13 @@
         <v>204</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="M103" s="7" t="s">
-        <v>325</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -4678,13 +4749,13 @@
         <v>204</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M104" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -4692,13 +4763,13 @@
         <v>204</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="M105" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -4706,13 +4777,13 @@
         <v>204</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="M106" s="7" t="s">
-        <v>330</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -4720,13 +4791,13 @@
         <v>204</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="M107" s="7" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -4734,19 +4805,13 @@
         <v>204</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="H108" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="I108" s="7" t="s">
-        <v>404</v>
+        <v>331</v>
       </c>
       <c r="M108" s="7" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -4754,19 +4819,13 @@
         <v>204</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="H109" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="I109" s="12" t="s">
-        <v>405</v>
+        <v>332</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -4774,13 +4833,19 @@
         <v>204</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>404</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -4788,13 +4853,19 @@
         <v>204</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="I111" s="12" t="s">
+        <v>405</v>
       </c>
       <c r="M111" s="7" t="s">
-        <v>335</v>
+        <v>254</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -4802,13 +4873,13 @@
         <v>204</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="M112" s="8" t="s">
-        <v>260</v>
+        <v>334</v>
+      </c>
+      <c r="M112" s="7" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -4816,13 +4887,13 @@
         <v>204</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M113" s="7" t="s">
-        <v>262</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -4830,13 +4901,13 @@
         <v>204</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>339</v>
+        <v>261</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>342</v>
+        <v>260</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -4844,13 +4915,13 @@
         <v>204</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M115" s="8" t="s">
-        <v>343</v>
+        <v>338</v>
+      </c>
+      <c r="M115" s="7" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -4858,19 +4929,13 @@
         <v>204</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="H116" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="I116" s="7" t="s">
-        <v>408</v>
+        <v>339</v>
       </c>
       <c r="M116" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -4878,18 +4943,52 @@
         <v>204</v>
       </c>
       <c r="B117" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="H118" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="I118" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="M118" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="C119" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="H117" s="7" t="s">
+      <c r="H119" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="I117" s="12" t="s">
+      <c r="I119" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="M117" s="8" t="s">
+      <c r="M119" s="8" t="s">
         <v>344</v>
       </c>
     </row>

</xml_diff>